<commit_message>
fully updated analyses on all participants; started developing RSA analysis
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_Combined.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_Combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179BC7EF-128A-4CBE-81F6-3C48CFBCD5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDF97EF-83E7-4148-B503-9F18F5D292F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>7,11,13,14,15,16,19</t>
+  </si>
+  <si>
+    <t>10,13,14,17,18</t>
+  </si>
+  <si>
+    <t>4,5,9,12,17,19</t>
+  </si>
+  <si>
+    <t>5,9,13,14,18,19</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,6 +758,40 @@
         <v>30</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20250725</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>